<commit_message>
FIX FOR SF9 & SF10
-fix only 1 subject export
-fix sf9 template format
-fix not computing final grade
-fix not showing grades when have missing grade
</commit_message>
<xml_diff>
--- a/Project Files/Forms System (SHS)/templates/shs_sf9.xlsx
+++ b/Project Files/Forms System (SHS)/templates/shs_sf9.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrmil\Documents\GitHub\CBNHS-System-SHS\Project Files\Forms System (SHS)\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F4D476-0752-414B-8812-A26490FD52C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC80A33-0E1D-41C7-9FE5-CE5B9430F847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="865" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FRONT" sheetId="149" r:id="rId1"/>
@@ -567,12 +567,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aparajita"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -598,6 +592,12 @@
       <u/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Aparajita"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aparajita"/>
       <family val="1"/>
     </font>
@@ -628,7 +628,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="70">
     <border>
       <left/>
       <right/>
@@ -745,7 +745,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -757,97 +757,22 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -1074,94 +999,512 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1169,7 +1512,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="186">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1251,58 +1594,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1321,39 +1634,103 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" textRotation="90"/>
@@ -1363,37 +1740,27 @@
       <alignment horizontal="center" textRotation="90"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1407,13 +1774,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="distributed" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="distributed" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1432,59 +1793,83 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90"/>
-      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1492,143 +1877,179 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1997,7 +2418,7 @@
   <sheetPr codeName="Sheet128"/>
   <dimension ref="A3:AA41"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <selection activeCell="T3" sqref="T3:U3"/>
     </sheetView>
   </sheetViews>
@@ -2021,71 +2442,71 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
-      <c r="L3" s="74"/>
-      <c r="M3" s="74"/>
-      <c r="N3" s="74"/>
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="104"/>
       <c r="O3" s="1"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="1"/>
       <c r="S3" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="T3" s="156"/>
-      <c r="U3" s="156"/>
+      <c r="T3" s="112"/>
+      <c r="U3" s="112"/>
     </row>
     <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="75"/>
-      <c r="B4" s="77" t="s">
+      <c r="A4" s="105"/>
+      <c r="B4" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="107" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="77" t="s">
+      <c r="D4" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="77" t="s">
+      <c r="E4" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="77" t="s">
+      <c r="F4" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="77" t="s">
+      <c r="G4" s="107" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="77" t="s">
+      <c r="H4" s="107" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="77" t="s">
+      <c r="I4" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="77" t="s">
+      <c r="J4" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="77" t="s">
+      <c r="K4" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="77" t="s">
+      <c r="L4" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="81" t="s">
+      <c r="M4" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="84"/>
-      <c r="O4" s="84"/>
+      <c r="N4" s="103"/>
+      <c r="O4" s="103"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="33"/>
       <c r="R4" s="33"/>
@@ -2094,224 +2515,224 @@
       <c r="U4" s="5"/>
     </row>
     <row r="5" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="76"/>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="82"/>
-      <c r="N5" s="84"/>
-      <c r="O5" s="84"/>
-      <c r="P5" s="55"/>
-      <c r="Q5" s="70" t="s">
+      <c r="A5" s="106"/>
+      <c r="B5" s="108"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="108"/>
+      <c r="G5" s="108"/>
+      <c r="H5" s="108"/>
+      <c r="I5" s="108"/>
+      <c r="J5" s="108"/>
+      <c r="K5" s="108"/>
+      <c r="L5" s="108"/>
+      <c r="M5" s="101"/>
+      <c r="N5" s="103"/>
+      <c r="O5" s="103"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="91" t="s">
         <v>83</v>
       </c>
-      <c r="R5" s="70"/>
-      <c r="S5" s="70"/>
-      <c r="T5" s="70"/>
-      <c r="U5" s="55"/>
+      <c r="R5" s="91"/>
+      <c r="S5" s="91"/>
+      <c r="T5" s="91"/>
+      <c r="U5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="76"/>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="80"/>
-      <c r="H6" s="80"/>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="79"/>
-      <c r="L6" s="79"/>
-      <c r="M6" s="83"/>
-      <c r="N6" s="84"/>
-      <c r="O6" s="84"/>
-      <c r="P6" s="56"/>
-      <c r="Q6" s="68" t="s">
+      <c r="A6" s="106"/>
+      <c r="B6" s="109"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="110"/>
+      <c r="H6" s="110"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="109"/>
+      <c r="M6" s="102"/>
+      <c r="N6" s="103"/>
+      <c r="O6" s="103"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="114" t="s">
         <v>84</v>
       </c>
-      <c r="R6" s="68"/>
-      <c r="S6" s="68"/>
-      <c r="T6" s="68"/>
-      <c r="U6" s="56"/>
+      <c r="R6" s="114"/>
+      <c r="S6" s="114"/>
+      <c r="T6" s="114"/>
+      <c r="U6" s="46"/>
     </row>
     <row r="7" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="111" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="95"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="72"/>
-      <c r="L7" s="72"/>
-      <c r="M7" s="72"/>
-      <c r="N7" s="84"/>
-      <c r="O7" s="84"/>
-      <c r="P7" s="87"/>
-      <c r="Q7" s="158" t="s">
+      <c r="B7" s="83"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="83"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
+      <c r="L7" s="83"/>
+      <c r="M7" s="83"/>
+      <c r="N7" s="103"/>
+      <c r="O7" s="103"/>
+      <c r="P7" s="94"/>
+      <c r="Q7" s="113" t="s">
         <v>119</v>
       </c>
-      <c r="R7" s="158"/>
-      <c r="S7" s="158"/>
-      <c r="T7" s="158"/>
-      <c r="U7" s="55"/>
+      <c r="R7" s="113"/>
+      <c r="S7" s="113"/>
+      <c r="T7" s="113"/>
+      <c r="U7" s="45"/>
     </row>
     <row r="8" spans="1:23" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="71"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="73"/>
-      <c r="I8" s="73"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="73"/>
-      <c r="L8" s="73"/>
-      <c r="M8" s="73"/>
-      <c r="N8" s="84"/>
-      <c r="O8" s="84"/>
-      <c r="P8" s="87"/>
-      <c r="Q8" s="69" t="s">
+      <c r="A8" s="111"/>
+      <c r="B8" s="84"/>
+      <c r="C8" s="84"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="84"/>
+      <c r="F8" s="84"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="84"/>
+      <c r="J8" s="84"/>
+      <c r="K8" s="84"/>
+      <c r="L8" s="84"/>
+      <c r="M8" s="84"/>
+      <c r="N8" s="103"/>
+      <c r="O8" s="103"/>
+      <c r="P8" s="94"/>
+      <c r="Q8" s="115" t="s">
         <v>85</v>
       </c>
-      <c r="R8" s="69"/>
-      <c r="S8" s="69"/>
-      <c r="T8" s="69"/>
-      <c r="U8" s="55"/>
+      <c r="R8" s="115"/>
+      <c r="S8" s="115"/>
+      <c r="T8" s="115"/>
+      <c r="U8" s="45"/>
     </row>
     <row r="9" spans="1:23" ht="3.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="88" t="s">
+      <c r="A9" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="85"/>
-      <c r="C9" s="91"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="85"/>
-      <c r="I9" s="85"/>
-      <c r="J9" s="85"/>
-      <c r="K9" s="85"/>
-      <c r="L9" s="85"/>
-      <c r="M9" s="85"/>
-      <c r="P9" s="87"/>
-      <c r="Q9" s="57"/>
-      <c r="R9" s="57"/>
-      <c r="S9" s="57"/>
-      <c r="T9" s="57"/>
-      <c r="U9" s="55"/>
+      <c r="B9" s="92"/>
+      <c r="C9" s="96"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="92"/>
+      <c r="I9" s="92"/>
+      <c r="J9" s="92"/>
+      <c r="K9" s="92"/>
+      <c r="L9" s="92"/>
+      <c r="M9" s="92"/>
+      <c r="P9" s="94"/>
+      <c r="Q9" s="47"/>
+      <c r="R9" s="47"/>
+      <c r="S9" s="47"/>
+      <c r="T9" s="47"/>
+      <c r="U9" s="45"/>
     </row>
     <row r="10" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="89"/>
-      <c r="B10" s="86"/>
-      <c r="C10" s="92"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="86"/>
-      <c r="J10" s="86"/>
-      <c r="K10" s="86"/>
-      <c r="L10" s="86"/>
-      <c r="M10" s="86"/>
-      <c r="P10" s="58"/>
-      <c r="Q10" s="158" t="s">
+      <c r="A10" s="95"/>
+      <c r="B10" s="93"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="93"/>
+      <c r="F10" s="93"/>
+      <c r="G10" s="93"/>
+      <c r="H10" s="93"/>
+      <c r="I10" s="93"/>
+      <c r="J10" s="93"/>
+      <c r="K10" s="93"/>
+      <c r="L10" s="93"/>
+      <c r="M10" s="93"/>
+      <c r="P10" s="48"/>
+      <c r="Q10" s="113" t="s">
         <v>120</v>
       </c>
-      <c r="R10" s="158"/>
-      <c r="S10" s="158"/>
-      <c r="T10" s="158"/>
-      <c r="U10" s="55"/>
+      <c r="R10" s="113"/>
+      <c r="S10" s="113"/>
+      <c r="T10" s="113"/>
+      <c r="U10" s="45"/>
     </row>
     <row r="11" spans="1:23" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="90"/>
-      <c r="B11" s="86"/>
-      <c r="C11" s="93"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="94"/>
-      <c r="H11" s="94"/>
-      <c r="I11" s="86"/>
-      <c r="J11" s="86"/>
-      <c r="K11" s="86"/>
-      <c r="L11" s="86"/>
-      <c r="M11" s="86"/>
-      <c r="P11" s="55"/>
-      <c r="Q11" s="68" t="s">
+      <c r="A11" s="88"/>
+      <c r="B11" s="93"/>
+      <c r="C11" s="98"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="93"/>
+      <c r="F11" s="93"/>
+      <c r="G11" s="99"/>
+      <c r="H11" s="99"/>
+      <c r="I11" s="93"/>
+      <c r="J11" s="93"/>
+      <c r="K11" s="93"/>
+      <c r="L11" s="93"/>
+      <c r="M11" s="93"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="114" t="s">
         <v>82</v>
       </c>
-      <c r="R11" s="68"/>
-      <c r="S11" s="68"/>
-      <c r="T11" s="68"/>
-      <c r="U11" s="55"/>
+      <c r="R11" s="114"/>
+      <c r="S11" s="114"/>
+      <c r="T11" s="114"/>
+      <c r="U11" s="45"/>
     </row>
     <row r="12" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="97"/>
-      <c r="C12" s="97"/>
-      <c r="D12" s="97"/>
-      <c r="E12" s="97"/>
-      <c r="F12" s="97"/>
-      <c r="G12" s="98"/>
-      <c r="H12" s="98"/>
-      <c r="I12" s="97"/>
-      <c r="J12" s="97"/>
-      <c r="K12" s="97"/>
-      <c r="L12" s="97"/>
-      <c r="M12" s="97"/>
-      <c r="P12" s="159" t="s">
+      <c r="B12" s="81"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="89"/>
+      <c r="H12" s="89"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="81"/>
+      <c r="L12" s="81"/>
+      <c r="M12" s="81"/>
+      <c r="P12" s="90" t="s">
         <v>121</v>
       </c>
-      <c r="Q12" s="70"/>
-      <c r="R12" s="70"/>
-      <c r="S12" s="70"/>
-      <c r="T12" s="70"/>
-      <c r="U12" s="70"/>
+      <c r="Q12" s="91"/>
+      <c r="R12" s="91"/>
+      <c r="S12" s="91"/>
+      <c r="T12" s="91"/>
+      <c r="U12" s="91"/>
     </row>
     <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="90"/>
-      <c r="B13" s="97"/>
-      <c r="C13" s="97"/>
-      <c r="D13" s="97"/>
-      <c r="E13" s="97"/>
-      <c r="F13" s="97"/>
-      <c r="G13" s="97"/>
-      <c r="H13" s="97"/>
-      <c r="I13" s="97"/>
-      <c r="J13" s="97"/>
-      <c r="K13" s="97"/>
-      <c r="L13" s="97"/>
-      <c r="M13" s="97"/>
-      <c r="P13" s="55"/>
-      <c r="Q13" s="96" t="s">
+      <c r="A13" s="88"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="81"/>
+      <c r="K13" s="81"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="81"/>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="R13" s="96"/>
-      <c r="S13" s="96"/>
-      <c r="T13" s="96"/>
-      <c r="U13" s="55"/>
-      <c r="W13" s="59"/>
+      <c r="R13" s="86"/>
+      <c r="S13" s="86"/>
+      <c r="T13" s="86"/>
+      <c r="U13" s="45"/>
+      <c r="W13" s="49"/>
     </row>
     <row r="14" spans="1:23" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="28"/>
@@ -2346,31 +2767,31 @@
       <c r="Q15" s="8"/>
     </row>
     <row r="16" spans="1:23" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="99" t="s">
+      <c r="A16" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="99"/>
-      <c r="C16" s="99"/>
-      <c r="D16" s="99"/>
-      <c r="E16" s="99"/>
-      <c r="F16" s="99"/>
-      <c r="G16" s="99"/>
-      <c r="H16" s="99"/>
-      <c r="I16" s="99"/>
-      <c r="J16" s="99"/>
-      <c r="K16" s="99"/>
-      <c r="L16" s="99"/>
-      <c r="M16" s="99"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="78"/>
+      <c r="I16" s="78"/>
+      <c r="J16" s="78"/>
+      <c r="K16" s="78"/>
+      <c r="L16" s="78"/>
+      <c r="M16" s="78"/>
     </row>
     <row r="17" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P17" s="100" t="s">
+      <c r="P17" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="Q17" s="100"/>
-      <c r="R17" s="100"/>
-      <c r="S17" s="100"/>
-      <c r="T17" s="100"/>
-      <c r="U17" s="100"/>
+      <c r="Q17" s="82"/>
+      <c r="R17" s="82"/>
+      <c r="S17" s="82"/>
+      <c r="T17" s="82"/>
+      <c r="U17" s="82"/>
     </row>
     <row r="18" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="9" t="s">
@@ -2477,14 +2898,14 @@
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
-      <c r="P22" s="61" t="s">
+      <c r="P22" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="Q22" s="61"/>
-      <c r="R22" s="61"/>
-      <c r="S22" s="61"/>
-      <c r="T22" s="61"/>
-      <c r="U22" s="61"/>
+      <c r="Q22" s="51"/>
+      <c r="R22" s="51"/>
+      <c r="S22" s="51"/>
+      <c r="T22" s="51"/>
+      <c r="U22" s="51"/>
       <c r="X22" s="3" t="s">
         <v>61</v>
       </c>
@@ -2498,12 +2919,12 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
-      <c r="P23" s="60"/>
-      <c r="Q23" s="60"/>
-      <c r="R23" s="60"/>
-      <c r="S23" s="60"/>
-      <c r="T23" s="60"/>
-      <c r="U23" s="60"/>
+      <c r="P23" s="50"/>
+      <c r="Q23" s="50"/>
+      <c r="R23" s="50"/>
+      <c r="S23" s="50"/>
+      <c r="T23" s="50"/>
+      <c r="U23" s="50"/>
       <c r="X23" t="s">
         <v>70</v>
       </c>
@@ -2525,16 +2946,16 @@
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
       <c r="M24" s="13"/>
-      <c r="P24" s="61" t="s">
+      <c r="P24" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="Q24" s="61"/>
-      <c r="R24" s="61"/>
-      <c r="S24" s="61" t="s">
+      <c r="Q24" s="51"/>
+      <c r="R24" s="51"/>
+      <c r="S24" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="T24" s="61"/>
-      <c r="U24" s="61"/>
+      <c r="T24" s="51"/>
+      <c r="U24" s="51"/>
       <c r="X24" s="3" t="s">
         <v>62</v>
       </c>
@@ -2554,12 +2975,12 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
-      <c r="P25" s="60"/>
-      <c r="Q25" s="60"/>
-      <c r="R25" s="60"/>
-      <c r="S25" s="60"/>
-      <c r="T25" s="60"/>
-      <c r="U25" s="60"/>
+      <c r="P25" s="50"/>
+      <c r="Q25" s="50"/>
+      <c r="R25" s="50"/>
+      <c r="S25" s="50"/>
+      <c r="T25" s="50"/>
+      <c r="U25" s="50"/>
       <c r="X25" t="s">
         <v>63</v>
       </c>
@@ -2569,30 +2990,30 @@
       </c>
     </row>
     <row r="26" spans="1:26" ht="18" x14ac:dyDescent="0.4">
-      <c r="B26" s="101" t="s">
+      <c r="B26" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="101"/>
-      <c r="D26" s="101"/>
-      <c r="E26" s="101"/>
-      <c r="F26" s="101"/>
-      <c r="G26" s="101"/>
-      <c r="H26" s="101"/>
-      <c r="I26" s="101"/>
-      <c r="J26" s="101"/>
-      <c r="K26" s="101"/>
-      <c r="L26" s="101"/>
-      <c r="M26" s="101"/>
-      <c r="P26" s="60" t="s">
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="75"/>
+      <c r="H26" s="75"/>
+      <c r="I26" s="75"/>
+      <c r="J26" s="75"/>
+      <c r="K26" s="75"/>
+      <c r="L26" s="75"/>
+      <c r="M26" s="75"/>
+      <c r="P26" s="50" t="s">
         <v>115</v>
       </c>
-      <c r="Q26" s="60"/>
-      <c r="R26" s="60" t="s">
+      <c r="Q26" s="50"/>
+      <c r="R26" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="S26" s="60"/>
-      <c r="T26" s="60"/>
-      <c r="U26" s="60"/>
+      <c r="S26" s="50"/>
+      <c r="T26" s="50"/>
+      <c r="U26" s="50"/>
       <c r="X26" s="3" t="s">
         <v>64</v>
       </c>
@@ -2602,26 +3023,26 @@
       </c>
     </row>
     <row r="27" spans="1:26" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="102"/>
-      <c r="C27" s="102"/>
-      <c r="D27" s="102"/>
-      <c r="E27" s="102"/>
-      <c r="F27" s="102"/>
-      <c r="G27" s="102"/>
-      <c r="H27" s="102"/>
-      <c r="I27" s="102"/>
-      <c r="J27" s="102"/>
-      <c r="K27" s="102"/>
-      <c r="L27" s="102"/>
-      <c r="M27" s="102"/>
-      <c r="P27" s="61" t="s">
+      <c r="B27" s="79"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="79"/>
+      <c r="H27" s="79"/>
+      <c r="I27" s="79"/>
+      <c r="J27" s="79"/>
+      <c r="K27" s="79"/>
+      <c r="L27" s="79"/>
+      <c r="M27" s="79"/>
+      <c r="P27" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="Q27" s="157"/>
-      <c r="R27" s="157"/>
-      <c r="S27" s="157"/>
-      <c r="T27" s="157"/>
-      <c r="U27" s="157"/>
+      <c r="Q27" s="54"/>
+      <c r="R27" s="54"/>
+      <c r="S27" s="54"/>
+      <c r="T27" s="54"/>
+      <c r="U27" s="54"/>
       <c r="X27" s="18" t="s">
         <v>71</v>
       </c>
@@ -2647,14 +3068,14 @@
       <c r="L28" s="17"/>
       <c r="M28" s="17"/>
       <c r="N28" s="17"/>
-      <c r="P28" s="61" t="s">
+      <c r="P28" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="Q28" s="60"/>
-      <c r="R28" s="60"/>
-      <c r="S28" s="60"/>
-      <c r="T28" s="60"/>
-      <c r="U28" s="60"/>
+      <c r="Q28" s="50"/>
+      <c r="R28" s="50"/>
+      <c r="S28" s="50"/>
+      <c r="T28" s="50"/>
+      <c r="U28" s="50"/>
       <c r="X28" t="s">
         <v>65</v>
       </c>
@@ -2680,14 +3101,14 @@
       <c r="M29" s="19"/>
       <c r="N29" s="19"/>
       <c r="O29" s="9"/>
-      <c r="P29" s="61" t="s">
+      <c r="P29" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="Q29" s="61"/>
-      <c r="R29" s="61"/>
-      <c r="S29" s="61"/>
-      <c r="T29" s="61"/>
-      <c r="U29" s="61"/>
+      <c r="Q29" s="51"/>
+      <c r="R29" s="51"/>
+      <c r="S29" s="51"/>
+      <c r="T29" s="51"/>
+      <c r="U29" s="51"/>
       <c r="X29" s="3" t="s">
         <v>75</v>
       </c>
@@ -2789,21 +3210,21 @@
     </row>
     <row r="33" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="22"/>
-      <c r="B33" s="103" t="s">
+      <c r="B33" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="103"/>
-      <c r="D33" s="103"/>
+      <c r="C33" s="80"/>
+      <c r="D33" s="80"/>
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
       <c r="G33" s="1"/>
       <c r="H33" s="22"/>
       <c r="I33" s="22"/>
-      <c r="J33" s="103" t="s">
+      <c r="J33" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="K33" s="103"/>
-      <c r="L33" s="103"/>
+      <c r="K33" s="80"/>
+      <c r="L33" s="80"/>
       <c r="M33" s="22"/>
       <c r="N33" s="22"/>
       <c r="O33" s="1"/>
@@ -2817,29 +3238,29 @@
       <c r="U33" s="17"/>
     </row>
     <row r="34" spans="1:21" s="3" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="104" t="s">
+      <c r="A34" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="104"/>
-      <c r="C34" s="104"/>
-      <c r="D34" s="104"/>
-      <c r="E34" s="104"/>
-      <c r="F34" s="104"/>
+      <c r="B34" s="76"/>
+      <c r="C34" s="76"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="76"/>
       <c r="G34" s="9"/>
-      <c r="H34" s="104" t="s">
+      <c r="H34" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="I34" s="104"/>
-      <c r="J34" s="104"/>
-      <c r="K34" s="104"/>
-      <c r="L34" s="104"/>
-      <c r="M34" s="104"/>
-      <c r="N34" s="104"/>
+      <c r="I34" s="76"/>
+      <c r="J34" s="76"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="76"/>
+      <c r="M34" s="76"/>
+      <c r="N34" s="76"/>
       <c r="O34" s="9"/>
-      <c r="P34" s="105" t="s">
+      <c r="P34" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="Q34" s="105"/>
+      <c r="Q34" s="77"/>
       <c r="R34" s="15"/>
       <c r="S34" s="15"/>
       <c r="T34" s="15"/>
@@ -2856,20 +3277,20 @@
       <c r="U35" s="17"/>
     </row>
     <row r="36" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="99"/>
-      <c r="B36" s="99"/>
-      <c r="C36" s="99"/>
-      <c r="D36" s="99"/>
-      <c r="E36" s="99"/>
-      <c r="F36" s="99"/>
-      <c r="G36" s="99"/>
-      <c r="H36" s="99"/>
-      <c r="I36" s="99"/>
-      <c r="J36" s="99"/>
-      <c r="K36" s="99"/>
-      <c r="L36" s="99"/>
-      <c r="M36" s="99"/>
-      <c r="N36" s="99"/>
+      <c r="A36" s="78"/>
+      <c r="B36" s="78"/>
+      <c r="C36" s="78"/>
+      <c r="D36" s="78"/>
+      <c r="E36" s="78"/>
+      <c r="F36" s="78"/>
+      <c r="G36" s="78"/>
+      <c r="H36" s="78"/>
+      <c r="I36" s="78"/>
+      <c r="J36" s="78"/>
+      <c r="K36" s="78"/>
+      <c r="L36" s="78"/>
+      <c r="M36" s="78"/>
+      <c r="N36" s="78"/>
       <c r="P36" s="14" t="s">
         <v>32</v>
       </c>
@@ -2880,22 +3301,22 @@
       <c r="U36" s="17"/>
     </row>
     <row r="37" spans="1:21" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="101" t="s">
+      <c r="A37" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="101"/>
-      <c r="C37" s="101"/>
-      <c r="D37" s="101"/>
-      <c r="E37" s="101"/>
-      <c r="F37" s="101"/>
-      <c r="G37" s="101"/>
-      <c r="H37" s="101"/>
-      <c r="I37" s="101"/>
-      <c r="J37" s="101"/>
-      <c r="K37" s="101"/>
-      <c r="L37" s="101"/>
-      <c r="M37" s="101"/>
-      <c r="N37" s="101"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="75"/>
+      <c r="H37" s="75"/>
+      <c r="I37" s="75"/>
+      <c r="J37" s="75"/>
+      <c r="K37" s="75"/>
+      <c r="L37" s="75"/>
+      <c r="M37" s="75"/>
+      <c r="N37" s="75"/>
       <c r="P37" s="25" t="s">
         <v>34</v>
       </c>
@@ -2958,16 +3379,16 @@
       <c r="L40" s="20"/>
       <c r="M40" s="20"/>
       <c r="N40" s="20"/>
-      <c r="P40" s="99" t="s">
+      <c r="P40" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="Q40" s="99"/>
-      <c r="R40" s="99"/>
-      <c r="S40" s="99" t="s">
+      <c r="Q40" s="78"/>
+      <c r="R40" s="78"/>
+      <c r="S40" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="T40" s="99"/>
-      <c r="U40" s="99"/>
+      <c r="T40" s="78"/>
+      <c r="U40" s="78"/>
     </row>
     <row r="41" spans="1:21" ht="18" x14ac:dyDescent="0.4">
       <c r="A41" s="23"/>
@@ -2986,38 +3407,66 @@
       <c r="L41" s="27"/>
       <c r="M41" s="27"/>
       <c r="N41" s="27"/>
-      <c r="P41" s="101" t="s">
+      <c r="P41" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="Q41" s="101"/>
-      <c r="R41" s="101"/>
-      <c r="S41" s="101" t="s">
+      <c r="Q41" s="75"/>
+      <c r="R41" s="75"/>
+      <c r="S41" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="T41" s="101"/>
-      <c r="U41" s="101"/>
+      <c r="T41" s="75"/>
+      <c r="U41" s="75"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="80">
-    <mergeCell ref="P41:R41"/>
-    <mergeCell ref="S41:U41"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="H34:N34"/>
-    <mergeCell ref="P34:Q34"/>
-    <mergeCell ref="A36:N36"/>
-    <mergeCell ref="A37:N37"/>
-    <mergeCell ref="P40:R40"/>
-    <mergeCell ref="B26:M26"/>
-    <mergeCell ref="B27:M27"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="S40:U40"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="A16:M16"/>
-    <mergeCell ref="P17:U17"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="Q10:T10"/>
+    <mergeCell ref="Q6:T6"/>
+    <mergeCell ref="Q8:T8"/>
+    <mergeCell ref="Q11:T11"/>
+    <mergeCell ref="Q5:T5"/>
+    <mergeCell ref="Q7:T7"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A3:N3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="K4:K6"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="N4:N8"/>
+    <mergeCell ref="O4:O8"/>
+    <mergeCell ref="M9:M11"/>
+    <mergeCell ref="P7:P9"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J9:J11"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="Q13:T13"/>
@@ -3034,52 +3483,24 @@
     <mergeCell ref="K9:K11"/>
     <mergeCell ref="L9:L11"/>
     <mergeCell ref="I12:I13"/>
-    <mergeCell ref="M9:M11"/>
-    <mergeCell ref="P7:P9"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="J9:J11"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="N4:N8"/>
-    <mergeCell ref="O4:O8"/>
-    <mergeCell ref="A3:N3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="I4:I6"/>
-    <mergeCell ref="J4:J6"/>
-    <mergeCell ref="K4:K6"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="Q10:T10"/>
-    <mergeCell ref="Q6:T6"/>
-    <mergeCell ref="Q8:T8"/>
-    <mergeCell ref="Q11:T11"/>
-    <mergeCell ref="Q5:T5"/>
-    <mergeCell ref="Q7:T7"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="A16:M16"/>
+    <mergeCell ref="P17:U17"/>
+    <mergeCell ref="B26:M26"/>
+    <mergeCell ref="B27:M27"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="S40:U40"/>
+    <mergeCell ref="P41:R41"/>
+    <mergeCell ref="S41:U41"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="H34:N34"/>
+    <mergeCell ref="P34:Q34"/>
+    <mergeCell ref="A36:N36"/>
+    <mergeCell ref="A37:N37"/>
+    <mergeCell ref="P40:R40"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0" footer="0"/>
@@ -3093,8 +3514,8 @@
   <sheetPr codeName="Sheet127"/>
   <dimension ref="B2:N33"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="175" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:E19"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="175" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="17.25" x14ac:dyDescent="0.4"/>
@@ -3113,573 +3534,527 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="133" t="s">
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="131" t="s">
         <v>94</v>
       </c>
-      <c r="H2" s="133"/>
-      <c r="I2" s="133"/>
-      <c r="J2" s="133"/>
-      <c r="K2" s="133"/>
-      <c r="L2" s="133"/>
-      <c r="M2" s="133"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131"/>
+      <c r="M2" s="131"/>
     </row>
     <row r="3" spans="2:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="136" t="s">
+      <c r="B3" s="161" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="136"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="136"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="161"/>
+      <c r="E3" s="161"/>
     </row>
     <row r="4" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="139" t="s">
+      <c r="B4" s="119" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="141" t="s">
+      <c r="C4" s="121" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="142"/>
-      <c r="E4" s="42" t="s">
+      <c r="D4" s="122"/>
+      <c r="E4" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="G4" s="146" t="s">
+      <c r="G4" s="144" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="131" t="s">
+      <c r="H4" s="171" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="131"/>
-      <c r="J4" s="131" t="s">
+      <c r="I4" s="172"/>
+      <c r="J4" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="131"/>
-      <c r="L4" s="131"/>
-      <c r="M4" s="148"/>
+      <c r="K4" s="142"/>
+      <c r="L4" s="142"/>
+      <c r="M4" s="143"/>
     </row>
     <row r="5" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="140"/>
-      <c r="C5" s="67">
+      <c r="B5" s="120"/>
+      <c r="C5" s="53">
         <v>1</v>
       </c>
-      <c r="D5" s="67">
+      <c r="D5" s="53">
         <v>2</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="G5" s="147"/>
-      <c r="H5" s="132"/>
-      <c r="I5" s="132"/>
-      <c r="J5" s="37">
+      <c r="G5" s="145"/>
+      <c r="H5" s="173"/>
+      <c r="I5" s="174"/>
+      <c r="J5" s="65">
         <v>1</v>
       </c>
-      <c r="K5" s="37">
+      <c r="K5" s="65">
         <v>2</v>
       </c>
-      <c r="L5" s="37">
+      <c r="L5" s="65">
         <v>3</v>
       </c>
-      <c r="M5" s="39">
+      <c r="M5" s="66">
         <v>4</v>
       </c>
-      <c r="N5" s="49"/>
-    </row>
-    <row r="6" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="64"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="66"/>
-      <c r="G6" s="135" t="s">
+      <c r="N5" s="68"/>
+    </row>
+    <row r="6" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="52"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="56"/>
+      <c r="G6" s="162" t="s">
         <v>107</v>
       </c>
-      <c r="H6" s="134" t="s">
+      <c r="H6" s="167" t="s">
         <v>108</v>
       </c>
-      <c r="I6" s="134"/>
-      <c r="J6" s="112"/>
-      <c r="K6" s="112"/>
-      <c r="L6" s="112"/>
-      <c r="M6" s="114"/>
-    </row>
-    <row r="7" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="44"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="45"/>
-      <c r="G7" s="135"/>
-      <c r="H7" s="134"/>
-      <c r="I7" s="134"/>
-      <c r="J7" s="113"/>
-      <c r="K7" s="113"/>
-      <c r="L7" s="113"/>
-      <c r="M7" s="115"/>
-    </row>
-    <row r="8" spans="2:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="44"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="45"/>
-      <c r="G8" s="135"/>
-      <c r="H8" s="134" t="s">
+      <c r="I6" s="168"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="126"/>
+      <c r="L6" s="126"/>
+      <c r="M6" s="124"/>
+    </row>
+    <row r="7" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="40"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="57"/>
+      <c r="G7" s="163"/>
+      <c r="H7" s="169"/>
+      <c r="I7" s="170"/>
+      <c r="J7" s="127"/>
+      <c r="K7" s="127"/>
+      <c r="L7" s="127"/>
+      <c r="M7" s="125"/>
+    </row>
+    <row r="8" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="41"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="59"/>
+      <c r="G8" s="164"/>
+      <c r="H8" s="165" t="s">
         <v>95</v>
       </c>
-      <c r="I8" s="134"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="40"/>
-    </row>
-    <row r="9" spans="2:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="46"/>
-      <c r="C9" s="149"/>
-      <c r="D9" s="149"/>
-      <c r="E9" s="151"/>
-      <c r="G9" s="123" t="s">
+      <c r="I8" s="166"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="37"/>
+    </row>
+    <row r="9" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="69"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="71"/>
+      <c r="G9" s="139" t="s">
         <v>96</v>
       </c>
-      <c r="H9" s="138" t="s">
+      <c r="H9" s="135" t="s">
         <v>97</v>
       </c>
-      <c r="I9" s="138"/>
-      <c r="J9" s="112"/>
-      <c r="K9" s="112"/>
-      <c r="L9" s="112"/>
-      <c r="M9" s="114"/>
-    </row>
-    <row r="10" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="47"/>
-      <c r="C10" s="150"/>
-      <c r="D10" s="150"/>
-      <c r="E10" s="152"/>
-      <c r="G10" s="123"/>
-      <c r="H10" s="138"/>
+      <c r="I9" s="136"/>
+      <c r="J9" s="126"/>
+      <c r="K9" s="126"/>
+      <c r="L9" s="126"/>
+      <c r="M9" s="124"/>
+    </row>
+    <row r="10" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="72"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="74"/>
+      <c r="G10" s="146"/>
+      <c r="H10" s="137"/>
       <c r="I10" s="138"/>
-      <c r="J10" s="113"/>
-      <c r="K10" s="113"/>
-      <c r="L10" s="113"/>
-      <c r="M10" s="115"/>
-    </row>
-    <row r="11" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="44"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="45"/>
-      <c r="G11" s="123"/>
-      <c r="H11" s="138" t="s">
+      <c r="J10" s="127"/>
+      <c r="K10" s="127"/>
+      <c r="L10" s="127"/>
+      <c r="M10" s="125"/>
+    </row>
+    <row r="11" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="40"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="57"/>
+      <c r="G11" s="146"/>
+      <c r="H11" s="135" t="s">
         <v>109</v>
       </c>
-      <c r="I11" s="138"/>
-      <c r="J11" s="112"/>
-      <c r="K11" s="112"/>
-      <c r="L11" s="112"/>
-      <c r="M11" s="114"/>
-    </row>
-    <row r="12" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="44"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="45"/>
-      <c r="G12" s="123"/>
-      <c r="H12" s="138"/>
+      <c r="I11" s="136"/>
+      <c r="J11" s="126"/>
+      <c r="K11" s="126"/>
+      <c r="L11" s="126"/>
+      <c r="M11" s="124"/>
+    </row>
+    <row r="12" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="40"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="57"/>
+      <c r="G12" s="140"/>
+      <c r="H12" s="137"/>
       <c r="I12" s="138"/>
-      <c r="J12" s="113"/>
-      <c r="K12" s="113"/>
-      <c r="L12" s="113"/>
-      <c r="M12" s="115"/>
-    </row>
-    <row r="13" spans="2:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="44"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="45"/>
-      <c r="G13" s="123" t="s">
+      <c r="J12" s="127"/>
+      <c r="K12" s="127"/>
+      <c r="L12" s="127"/>
+      <c r="M12" s="125"/>
+    </row>
+    <row r="13" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="40"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="57"/>
+      <c r="G13" s="139" t="s">
         <v>98</v>
       </c>
-      <c r="H13" s="138" t="s">
+      <c r="H13" s="135" t="s">
         <v>110</v>
       </c>
-      <c r="I13" s="138"/>
-      <c r="J13" s="112"/>
-      <c r="K13" s="112"/>
-      <c r="L13" s="112"/>
-      <c r="M13" s="114"/>
+      <c r="I13" s="136"/>
+      <c r="J13" s="126"/>
+      <c r="K13" s="126"/>
+      <c r="L13" s="126"/>
+      <c r="M13" s="124"/>
     </row>
     <row r="14" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="64"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="66"/>
-      <c r="G14" s="123"/>
-      <c r="H14" s="138"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="56"/>
+      <c r="G14" s="140"/>
+      <c r="H14" s="137"/>
       <c r="I14" s="138"/>
-      <c r="J14" s="113"/>
-      <c r="K14" s="113"/>
-      <c r="L14" s="113"/>
-      <c r="M14" s="115"/>
+      <c r="J14" s="127"/>
+      <c r="K14" s="127"/>
+      <c r="L14" s="127"/>
+      <c r="M14" s="125"/>
     </row>
     <row r="15" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="44"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="45"/>
-      <c r="G15" s="123" t="s">
+      <c r="B15" s="40"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="57"/>
+      <c r="G15" s="139" t="s">
         <v>99</v>
       </c>
-      <c r="H15" s="121" t="s">
+      <c r="H15" s="148" t="s">
         <v>100</v>
       </c>
-      <c r="I15" s="121"/>
-      <c r="J15" s="112"/>
-      <c r="K15" s="112"/>
-      <c r="L15" s="112"/>
-      <c r="M15" s="114"/>
-    </row>
-    <row r="16" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="44"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="45"/>
-      <c r="G16" s="123"/>
-      <c r="H16" s="121"/>
-      <c r="I16" s="121"/>
-      <c r="J16" s="137"/>
-      <c r="K16" s="137"/>
-      <c r="L16" s="137"/>
-      <c r="M16" s="155"/>
-    </row>
-    <row r="17" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="44"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="45"/>
-      <c r="G17" s="123"/>
-      <c r="H17" s="121"/>
-      <c r="I17" s="121"/>
-      <c r="J17" s="113"/>
-      <c r="K17" s="113"/>
-      <c r="L17" s="113"/>
-      <c r="M17" s="115"/>
+      <c r="I15" s="149"/>
+      <c r="J15" s="126"/>
+      <c r="K15" s="126"/>
+      <c r="L15" s="126"/>
+      <c r="M15" s="124"/>
+    </row>
+    <row r="16" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="40"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="57"/>
+      <c r="G16" s="146"/>
+      <c r="H16" s="152"/>
+      <c r="I16" s="153"/>
+      <c r="J16" s="130"/>
+      <c r="K16" s="130"/>
+      <c r="L16" s="130"/>
+      <c r="M16" s="129"/>
+    </row>
+    <row r="17" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="40"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="57"/>
+      <c r="G17" s="146"/>
+      <c r="H17" s="154"/>
+      <c r="I17" s="155"/>
+      <c r="J17" s="127"/>
+      <c r="K17" s="127"/>
+      <c r="L17" s="127"/>
+      <c r="M17" s="125"/>
     </row>
     <row r="18" spans="2:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="143" t="s">
+      <c r="B18" s="116" t="s">
         <v>106</v>
       </c>
-      <c r="C18" s="144"/>
-      <c r="D18" s="145"/>
-      <c r="E18" s="48"/>
-      <c r="G18" s="123"/>
-      <c r="H18" s="121" t="s">
+      <c r="C18" s="117"/>
+      <c r="D18" s="118"/>
+      <c r="E18" s="42"/>
+      <c r="G18" s="146"/>
+      <c r="H18" s="148" t="s">
         <v>111</v>
       </c>
-      <c r="I18" s="121"/>
-      <c r="J18" s="112"/>
-      <c r="K18" s="112"/>
-      <c r="L18" s="112"/>
-      <c r="M18" s="114"/>
+      <c r="I18" s="149"/>
+      <c r="J18" s="126"/>
+      <c r="K18" s="126"/>
+      <c r="L18" s="126"/>
+      <c r="M18" s="124"/>
     </row>
     <row r="19" spans="2:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="136" t="s">
+      <c r="B19" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="136"/>
-      <c r="D19" s="136"/>
-      <c r="E19" s="136"/>
-      <c r="G19" s="124"/>
-      <c r="H19" s="122"/>
-      <c r="I19" s="122"/>
-      <c r="J19" s="154"/>
-      <c r="K19" s="154"/>
-      <c r="L19" s="154"/>
-      <c r="M19" s="153"/>
+      <c r="C19" s="123"/>
+      <c r="D19" s="123"/>
+      <c r="E19" s="123"/>
+      <c r="G19" s="147"/>
+      <c r="H19" s="150"/>
+      <c r="I19" s="151"/>
+      <c r="J19" s="128"/>
+      <c r="K19" s="128"/>
+      <c r="L19" s="128"/>
+      <c r="M19" s="134"/>
     </row>
     <row r="20" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="139" t="s">
+      <c r="B20" s="119" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="141" t="s">
+      <c r="C20" s="121" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="142"/>
-      <c r="E20" s="42" t="s">
+      <c r="D20" s="122"/>
+      <c r="E20" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="G20" s="116" t="s">
+      <c r="G20" s="156" t="s">
         <v>101</v>
       </c>
-      <c r="H20" s="117"/>
-      <c r="I20" s="118"/>
+      <c r="H20" s="157"/>
+      <c r="I20" s="158"/>
     </row>
     <row r="21" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="140"/>
-      <c r="C21" s="67">
+      <c r="B21" s="120"/>
+      <c r="C21" s="53">
         <v>3</v>
       </c>
-      <c r="D21" s="67">
+      <c r="D21" s="53">
         <v>4</v>
       </c>
-      <c r="E21" s="43" t="s">
+      <c r="E21" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="41" t="s">
+      <c r="G21" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="H21" s="120" t="s">
+      <c r="H21" s="159" t="s">
         <v>102</v>
       </c>
-      <c r="I21" s="125"/>
-    </row>
-    <row r="22" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="64"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="65"/>
-      <c r="E22" s="66"/>
-      <c r="G22" s="50" t="s">
+      <c r="I21" s="160"/>
+    </row>
+    <row r="22" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="52"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="56"/>
+      <c r="G22" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="H22" s="106" t="s">
+      <c r="H22" s="132" t="s">
         <v>103</v>
       </c>
-      <c r="I22" s="107"/>
-    </row>
-    <row r="23" spans="2:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="44"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="45"/>
-      <c r="G23" s="50" t="s">
+      <c r="I22" s="133"/>
+    </row>
+    <row r="23" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="40"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="57"/>
+      <c r="G23" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="H23" s="106" t="s">
+      <c r="H23" s="132" t="s">
         <v>52</v>
       </c>
-      <c r="I23" s="107"/>
-    </row>
-    <row r="24" spans="2:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="44"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="45"/>
-      <c r="G24" s="50" t="s">
+      <c r="I23" s="133"/>
+    </row>
+    <row r="24" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="40"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="57"/>
+      <c r="G24" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="H24" s="106" t="s">
+      <c r="H24" s="132" t="s">
         <v>56</v>
       </c>
-      <c r="I24" s="107"/>
-    </row>
-    <row r="25" spans="2:13" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="44"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="45"/>
-      <c r="G25" s="53" t="s">
+      <c r="I24" s="133"/>
+    </row>
+    <row r="25" spans="2:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="40"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="57"/>
+      <c r="G25" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="H25" s="129" t="s">
+      <c r="H25" s="177" t="s">
         <v>60</v>
       </c>
-      <c r="I25" s="130"/>
-    </row>
-    <row r="26" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="44"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="45"/>
-      <c r="G26" s="126" t="s">
+      <c r="I25" s="178"/>
+    </row>
+    <row r="26" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="40"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="57"/>
+      <c r="G26" s="156" t="s">
         <v>104</v>
       </c>
-      <c r="H26" s="127"/>
-      <c r="I26" s="127"/>
-      <c r="J26" s="127"/>
-      <c r="K26" s="127"/>
-      <c r="L26" s="127"/>
-      <c r="M26" s="128"/>
-    </row>
-    <row r="27" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="44"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="45"/>
-      <c r="G27" s="119" t="s">
+      <c r="H26" s="157"/>
+      <c r="I26" s="157"/>
+      <c r="J26" s="157"/>
+      <c r="K26" s="157"/>
+      <c r="L26" s="157"/>
+      <c r="M26" s="158"/>
+    </row>
+    <row r="27" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="40"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="57"/>
+      <c r="G27" s="175" t="s">
         <v>105</v>
       </c>
-      <c r="H27" s="120"/>
-      <c r="I27" s="37" t="s">
+      <c r="H27" s="176"/>
+      <c r="I27" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="J27" s="120" t="s">
+      <c r="J27" s="159" t="s">
         <v>1</v>
       </c>
-      <c r="K27" s="120"/>
-      <c r="L27" s="120"/>
-      <c r="M27" s="125"/>
-    </row>
-    <row r="28" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="44"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="45"/>
-      <c r="G28" s="108" t="s">
+      <c r="K27" s="180"/>
+      <c r="L27" s="180"/>
+      <c r="M27" s="160"/>
+    </row>
+    <row r="28" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="40"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="57"/>
+      <c r="G28" s="181" t="s">
         <v>42</v>
       </c>
-      <c r="H28" s="106"/>
-      <c r="I28" s="51" t="s">
+      <c r="H28" s="182"/>
+      <c r="I28" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="J28" s="106" t="s">
+      <c r="J28" s="132" t="s">
         <v>44</v>
       </c>
-      <c r="K28" s="106"/>
-      <c r="L28" s="106"/>
-      <c r="M28" s="107"/>
-    </row>
-    <row r="29" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="64"/>
-      <c r="C29" s="65"/>
-      <c r="D29" s="65"/>
-      <c r="E29" s="66"/>
-      <c r="G29" s="108" t="s">
+      <c r="K28" s="179"/>
+      <c r="L28" s="179"/>
+      <c r="M28" s="133"/>
+    </row>
+    <row r="29" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B29" s="52"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="56"/>
+      <c r="G29" s="181" t="s">
         <v>46</v>
       </c>
-      <c r="H29" s="106"/>
-      <c r="I29" s="51" t="s">
+      <c r="H29" s="182"/>
+      <c r="I29" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="J29" s="106" t="s">
+      <c r="J29" s="132" t="s">
         <v>44</v>
       </c>
-      <c r="K29" s="106"/>
-      <c r="L29" s="106"/>
-      <c r="M29" s="107"/>
-    </row>
-    <row r="30" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="44"/>
-      <c r="C30" s="63"/>
-      <c r="D30" s="63"/>
-      <c r="E30" s="45"/>
-      <c r="G30" s="108" t="s">
+      <c r="K29" s="179"/>
+      <c r="L29" s="179"/>
+      <c r="M29" s="133"/>
+    </row>
+    <row r="30" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="40"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="57"/>
+      <c r="G30" s="181" t="s">
         <v>49</v>
       </c>
-      <c r="H30" s="106"/>
-      <c r="I30" s="51" t="s">
+      <c r="H30" s="182"/>
+      <c r="I30" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="J30" s="106" t="s">
+      <c r="J30" s="132" t="s">
         <v>44</v>
       </c>
-      <c r="K30" s="106"/>
-      <c r="L30" s="106"/>
-      <c r="M30" s="107"/>
-    </row>
-    <row r="31" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="44"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="45"/>
-      <c r="G31" s="108" t="s">
+      <c r="K30" s="179"/>
+      <c r="L30" s="179"/>
+      <c r="M30" s="133"/>
+    </row>
+    <row r="31" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="40"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="57"/>
+      <c r="G31" s="181" t="s">
         <v>53</v>
       </c>
-      <c r="H31" s="106"/>
-      <c r="I31" s="51" t="s">
+      <c r="H31" s="182"/>
+      <c r="I31" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="J31" s="106" t="s">
+      <c r="J31" s="132" t="s">
         <v>44</v>
       </c>
-      <c r="K31" s="106"/>
-      <c r="L31" s="106"/>
-      <c r="M31" s="107"/>
-    </row>
-    <row r="32" spans="2:13" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="44"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="45"/>
-      <c r="G32" s="111" t="s">
+      <c r="K31" s="179"/>
+      <c r="L31" s="179"/>
+      <c r="M31" s="133"/>
+    </row>
+    <row r="32" spans="2:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="40"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="57"/>
+      <c r="G32" s="183" t="s">
         <v>112</v>
       </c>
-      <c r="H32" s="109"/>
-      <c r="I32" s="52" t="s">
+      <c r="H32" s="184"/>
+      <c r="I32" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="J32" s="109" t="s">
+      <c r="J32" s="177" t="s">
         <v>58</v>
       </c>
-      <c r="K32" s="109"/>
-      <c r="L32" s="109"/>
-      <c r="M32" s="110"/>
+      <c r="K32" s="185"/>
+      <c r="L32" s="185"/>
+      <c r="M32" s="178"/>
     </row>
     <row r="33" spans="2:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B33" s="143" t="s">
+      <c r="B33" s="116" t="s">
         <v>106</v>
       </c>
-      <c r="C33" s="144"/>
-      <c r="D33" s="145"/>
-      <c r="E33" s="48"/>
+      <c r="C33" s="117"/>
+      <c r="D33" s="118"/>
+      <c r="E33" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="70">
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H11:I12"/>
-    <mergeCell ref="H13:I14"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="H9:I10"/>
-    <mergeCell ref="G9:G12"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="K15:K17"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="L13:L14"/>
+  <mergeCells count="67">
+    <mergeCell ref="J30:M30"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="J31:M31"/>
+    <mergeCell ref="J32:M32"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
     <mergeCell ref="J29:M29"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="M15:M17"/>
-    <mergeCell ref="L15:L17"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="H4:I5"/>
-    <mergeCell ref="G2:M2"/>
-    <mergeCell ref="H6:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G26:M26"/>
-    <mergeCell ref="J27:M27"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="H15:I17"/>
-    <mergeCell ref="H18:I19"/>
-    <mergeCell ref="G15:G19"/>
-    <mergeCell ref="H21:I21"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:K7"/>
@@ -3689,13 +4064,56 @@
     <mergeCell ref="L11:L12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J30:M30"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="J31:M31"/>
-    <mergeCell ref="J32:M32"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G26:M26"/>
+    <mergeCell ref="J27:M27"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G9:G12"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="H4:I5"/>
+    <mergeCell ref="G2:M2"/>
+    <mergeCell ref="H6:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="M15:M17"/>
+    <mergeCell ref="L15:L17"/>
+    <mergeCell ref="H9:I10"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="H15:I17"/>
+    <mergeCell ref="H18:I19"/>
+    <mergeCell ref="G15:G19"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H11:I12"/>
+    <mergeCell ref="H13:I14"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="J9:J10"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0" footer="0"/>

</xml_diff>

<commit_message>
Fix for SF9&10 w/ updated DB for student rankings
-added form_sf5_viewfull_shs
-fix sf9 template
-fix not loading empty records
-fix only 1 grade export issue
</commit_message>
<xml_diff>
--- a/Project Files/Forms System (SHS)/templates/shs_sf9.xlsx
+++ b/Project Files/Forms System (SHS)/templates/shs_sf9.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrmil\Documents\GitHub\CBNHS-System-SHS\Project Files\Forms System (SHS)\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F4D476-0752-414B-8812-A26490FD52C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC80A33-0E1D-41C7-9FE5-CE5B9430F847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="865" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FRONT" sheetId="149" r:id="rId1"/>
@@ -567,12 +567,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aparajita"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -598,6 +592,12 @@
       <u/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Aparajita"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aparajita"/>
       <family val="1"/>
     </font>
@@ -628,7 +628,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="70">
     <border>
       <left/>
       <right/>
@@ -745,7 +745,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -757,97 +757,22 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -1074,94 +999,512 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1169,7 +1512,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="186">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1251,58 +1594,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1321,39 +1634,103 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" textRotation="90"/>
@@ -1363,37 +1740,27 @@
       <alignment horizontal="center" textRotation="90"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1407,13 +1774,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="distributed" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="distributed" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1432,59 +1793,83 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90"/>
-      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1492,143 +1877,179 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1997,7 +2418,7 @@
   <sheetPr codeName="Sheet128"/>
   <dimension ref="A3:AA41"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <selection activeCell="T3" sqref="T3:U3"/>
     </sheetView>
   </sheetViews>
@@ -2021,71 +2442,71 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="74"/>
-      <c r="L3" s="74"/>
-      <c r="M3" s="74"/>
-      <c r="N3" s="74"/>
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="104"/>
       <c r="O3" s="1"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="1"/>
       <c r="S3" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="T3" s="156"/>
-      <c r="U3" s="156"/>
+      <c r="T3" s="112"/>
+      <c r="U3" s="112"/>
     </row>
     <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="75"/>
-      <c r="B4" s="77" t="s">
+      <c r="A4" s="105"/>
+      <c r="B4" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="107" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="77" t="s">
+      <c r="D4" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="77" t="s">
+      <c r="E4" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="77" t="s">
+      <c r="F4" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="77" t="s">
+      <c r="G4" s="107" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="77" t="s">
+      <c r="H4" s="107" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="77" t="s">
+      <c r="I4" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="77" t="s">
+      <c r="J4" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="77" t="s">
+      <c r="K4" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="77" t="s">
+      <c r="L4" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="81" t="s">
+      <c r="M4" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="84"/>
-      <c r="O4" s="84"/>
+      <c r="N4" s="103"/>
+      <c r="O4" s="103"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="33"/>
       <c r="R4" s="33"/>
@@ -2094,224 +2515,224 @@
       <c r="U4" s="5"/>
     </row>
     <row r="5" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="76"/>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="82"/>
-      <c r="N5" s="84"/>
-      <c r="O5" s="84"/>
-      <c r="P5" s="55"/>
-      <c r="Q5" s="70" t="s">
+      <c r="A5" s="106"/>
+      <c r="B5" s="108"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="108"/>
+      <c r="G5" s="108"/>
+      <c r="H5" s="108"/>
+      <c r="I5" s="108"/>
+      <c r="J5" s="108"/>
+      <c r="K5" s="108"/>
+      <c r="L5" s="108"/>
+      <c r="M5" s="101"/>
+      <c r="N5" s="103"/>
+      <c r="O5" s="103"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="91" t="s">
         <v>83</v>
       </c>
-      <c r="R5" s="70"/>
-      <c r="S5" s="70"/>
-      <c r="T5" s="70"/>
-      <c r="U5" s="55"/>
+      <c r="R5" s="91"/>
+      <c r="S5" s="91"/>
+      <c r="T5" s="91"/>
+      <c r="U5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="76"/>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="80"/>
-      <c r="H6" s="80"/>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="79"/>
-      <c r="L6" s="79"/>
-      <c r="M6" s="83"/>
-      <c r="N6" s="84"/>
-      <c r="O6" s="84"/>
-      <c r="P6" s="56"/>
-      <c r="Q6" s="68" t="s">
+      <c r="A6" s="106"/>
+      <c r="B6" s="109"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="110"/>
+      <c r="H6" s="110"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="109"/>
+      <c r="L6" s="109"/>
+      <c r="M6" s="102"/>
+      <c r="N6" s="103"/>
+      <c r="O6" s="103"/>
+      <c r="P6" s="46"/>
+      <c r="Q6" s="114" t="s">
         <v>84</v>
       </c>
-      <c r="R6" s="68"/>
-      <c r="S6" s="68"/>
-      <c r="T6" s="68"/>
-      <c r="U6" s="56"/>
+      <c r="R6" s="114"/>
+      <c r="S6" s="114"/>
+      <c r="T6" s="114"/>
+      <c r="U6" s="46"/>
     </row>
     <row r="7" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="111" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="95"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="72"/>
-      <c r="L7" s="72"/>
-      <c r="M7" s="72"/>
-      <c r="N7" s="84"/>
-      <c r="O7" s="84"/>
-      <c r="P7" s="87"/>
-      <c r="Q7" s="158" t="s">
+      <c r="B7" s="83"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="83"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
+      <c r="L7" s="83"/>
+      <c r="M7" s="83"/>
+      <c r="N7" s="103"/>
+      <c r="O7" s="103"/>
+      <c r="P7" s="94"/>
+      <c r="Q7" s="113" t="s">
         <v>119</v>
       </c>
-      <c r="R7" s="158"/>
-      <c r="S7" s="158"/>
-      <c r="T7" s="158"/>
-      <c r="U7" s="55"/>
+      <c r="R7" s="113"/>
+      <c r="S7" s="113"/>
+      <c r="T7" s="113"/>
+      <c r="U7" s="45"/>
     </row>
     <row r="8" spans="1:23" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="71"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="73"/>
-      <c r="I8" s="73"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="73"/>
-      <c r="L8" s="73"/>
-      <c r="M8" s="73"/>
-      <c r="N8" s="84"/>
-      <c r="O8" s="84"/>
-      <c r="P8" s="87"/>
-      <c r="Q8" s="69" t="s">
+      <c r="A8" s="111"/>
+      <c r="B8" s="84"/>
+      <c r="C8" s="84"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="84"/>
+      <c r="F8" s="84"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="84"/>
+      <c r="J8" s="84"/>
+      <c r="K8" s="84"/>
+      <c r="L8" s="84"/>
+      <c r="M8" s="84"/>
+      <c r="N8" s="103"/>
+      <c r="O8" s="103"/>
+      <c r="P8" s="94"/>
+      <c r="Q8" s="115" t="s">
         <v>85</v>
       </c>
-      <c r="R8" s="69"/>
-      <c r="S8" s="69"/>
-      <c r="T8" s="69"/>
-      <c r="U8" s="55"/>
+      <c r="R8" s="115"/>
+      <c r="S8" s="115"/>
+      <c r="T8" s="115"/>
+      <c r="U8" s="45"/>
     </row>
     <row r="9" spans="1:23" ht="3.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="88" t="s">
+      <c r="A9" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="85"/>
-      <c r="C9" s="91"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="85"/>
-      <c r="I9" s="85"/>
-      <c r="J9" s="85"/>
-      <c r="K9" s="85"/>
-      <c r="L9" s="85"/>
-      <c r="M9" s="85"/>
-      <c r="P9" s="87"/>
-      <c r="Q9" s="57"/>
-      <c r="R9" s="57"/>
-      <c r="S9" s="57"/>
-      <c r="T9" s="57"/>
-      <c r="U9" s="55"/>
+      <c r="B9" s="92"/>
+      <c r="C9" s="96"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="92"/>
+      <c r="I9" s="92"/>
+      <c r="J9" s="92"/>
+      <c r="K9" s="92"/>
+      <c r="L9" s="92"/>
+      <c r="M9" s="92"/>
+      <c r="P9" s="94"/>
+      <c r="Q9" s="47"/>
+      <c r="R9" s="47"/>
+      <c r="S9" s="47"/>
+      <c r="T9" s="47"/>
+      <c r="U9" s="45"/>
     </row>
     <row r="10" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="89"/>
-      <c r="B10" s="86"/>
-      <c r="C10" s="92"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="86"/>
-      <c r="J10" s="86"/>
-      <c r="K10" s="86"/>
-      <c r="L10" s="86"/>
-      <c r="M10" s="86"/>
-      <c r="P10" s="58"/>
-      <c r="Q10" s="158" t="s">
+      <c r="A10" s="95"/>
+      <c r="B10" s="93"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="93"/>
+      <c r="F10" s="93"/>
+      <c r="G10" s="93"/>
+      <c r="H10" s="93"/>
+      <c r="I10" s="93"/>
+      <c r="J10" s="93"/>
+      <c r="K10" s="93"/>
+      <c r="L10" s="93"/>
+      <c r="M10" s="93"/>
+      <c r="P10" s="48"/>
+      <c r="Q10" s="113" t="s">
         <v>120</v>
       </c>
-      <c r="R10" s="158"/>
-      <c r="S10" s="158"/>
-      <c r="T10" s="158"/>
-      <c r="U10" s="55"/>
+      <c r="R10" s="113"/>
+      <c r="S10" s="113"/>
+      <c r="T10" s="113"/>
+      <c r="U10" s="45"/>
     </row>
     <row r="11" spans="1:23" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="90"/>
-      <c r="B11" s="86"/>
-      <c r="C11" s="93"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="94"/>
-      <c r="H11" s="94"/>
-      <c r="I11" s="86"/>
-      <c r="J11" s="86"/>
-      <c r="K11" s="86"/>
-      <c r="L11" s="86"/>
-      <c r="M11" s="86"/>
-      <c r="P11" s="55"/>
-      <c r="Q11" s="68" t="s">
+      <c r="A11" s="88"/>
+      <c r="B11" s="93"/>
+      <c r="C11" s="98"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="93"/>
+      <c r="F11" s="93"/>
+      <c r="G11" s="99"/>
+      <c r="H11" s="99"/>
+      <c r="I11" s="93"/>
+      <c r="J11" s="93"/>
+      <c r="K11" s="93"/>
+      <c r="L11" s="93"/>
+      <c r="M11" s="93"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="114" t="s">
         <v>82</v>
       </c>
-      <c r="R11" s="68"/>
-      <c r="S11" s="68"/>
-      <c r="T11" s="68"/>
-      <c r="U11" s="55"/>
+      <c r="R11" s="114"/>
+      <c r="S11" s="114"/>
+      <c r="T11" s="114"/>
+      <c r="U11" s="45"/>
     </row>
     <row r="12" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="97"/>
-      <c r="C12" s="97"/>
-      <c r="D12" s="97"/>
-      <c r="E12" s="97"/>
-      <c r="F12" s="97"/>
-      <c r="G12" s="98"/>
-      <c r="H12" s="98"/>
-      <c r="I12" s="97"/>
-      <c r="J12" s="97"/>
-      <c r="K12" s="97"/>
-      <c r="L12" s="97"/>
-      <c r="M12" s="97"/>
-      <c r="P12" s="159" t="s">
+      <c r="B12" s="81"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="89"/>
+      <c r="H12" s="89"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="81"/>
+      <c r="L12" s="81"/>
+      <c r="M12" s="81"/>
+      <c r="P12" s="90" t="s">
         <v>121</v>
       </c>
-      <c r="Q12" s="70"/>
-      <c r="R12" s="70"/>
-      <c r="S12" s="70"/>
-      <c r="T12" s="70"/>
-      <c r="U12" s="70"/>
+      <c r="Q12" s="91"/>
+      <c r="R12" s="91"/>
+      <c r="S12" s="91"/>
+      <c r="T12" s="91"/>
+      <c r="U12" s="91"/>
     </row>
     <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="90"/>
-      <c r="B13" s="97"/>
-      <c r="C13" s="97"/>
-      <c r="D13" s="97"/>
-      <c r="E13" s="97"/>
-      <c r="F13" s="97"/>
-      <c r="G13" s="97"/>
-      <c r="H13" s="97"/>
-      <c r="I13" s="97"/>
-      <c r="J13" s="97"/>
-      <c r="K13" s="97"/>
-      <c r="L13" s="97"/>
-      <c r="M13" s="97"/>
-      <c r="P13" s="55"/>
-      <c r="Q13" s="96" t="s">
+      <c r="A13" s="88"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="81"/>
+      <c r="K13" s="81"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="81"/>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="R13" s="96"/>
-      <c r="S13" s="96"/>
-      <c r="T13" s="96"/>
-      <c r="U13" s="55"/>
-      <c r="W13" s="59"/>
+      <c r="R13" s="86"/>
+      <c r="S13" s="86"/>
+      <c r="T13" s="86"/>
+      <c r="U13" s="45"/>
+      <c r="W13" s="49"/>
     </row>
     <row r="14" spans="1:23" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="28"/>
@@ -2346,31 +2767,31 @@
       <c r="Q15" s="8"/>
     </row>
     <row r="16" spans="1:23" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="99" t="s">
+      <c r="A16" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="99"/>
-      <c r="C16" s="99"/>
-      <c r="D16" s="99"/>
-      <c r="E16" s="99"/>
-      <c r="F16" s="99"/>
-      <c r="G16" s="99"/>
-      <c r="H16" s="99"/>
-      <c r="I16" s="99"/>
-      <c r="J16" s="99"/>
-      <c r="K16" s="99"/>
-      <c r="L16" s="99"/>
-      <c r="M16" s="99"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="78"/>
+      <c r="I16" s="78"/>
+      <c r="J16" s="78"/>
+      <c r="K16" s="78"/>
+      <c r="L16" s="78"/>
+      <c r="M16" s="78"/>
     </row>
     <row r="17" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P17" s="100" t="s">
+      <c r="P17" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="Q17" s="100"/>
-      <c r="R17" s="100"/>
-      <c r="S17" s="100"/>
-      <c r="T17" s="100"/>
-      <c r="U17" s="100"/>
+      <c r="Q17" s="82"/>
+      <c r="R17" s="82"/>
+      <c r="S17" s="82"/>
+      <c r="T17" s="82"/>
+      <c r="U17" s="82"/>
     </row>
     <row r="18" spans="1:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="9" t="s">
@@ -2477,14 +2898,14 @@
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
-      <c r="P22" s="61" t="s">
+      <c r="P22" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="Q22" s="61"/>
-      <c r="R22" s="61"/>
-      <c r="S22" s="61"/>
-      <c r="T22" s="61"/>
-      <c r="U22" s="61"/>
+      <c r="Q22" s="51"/>
+      <c r="R22" s="51"/>
+      <c r="S22" s="51"/>
+      <c r="T22" s="51"/>
+      <c r="U22" s="51"/>
       <c r="X22" s="3" t="s">
         <v>61</v>
       </c>
@@ -2498,12 +2919,12 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
-      <c r="P23" s="60"/>
-      <c r="Q23" s="60"/>
-      <c r="R23" s="60"/>
-      <c r="S23" s="60"/>
-      <c r="T23" s="60"/>
-      <c r="U23" s="60"/>
+      <c r="P23" s="50"/>
+      <c r="Q23" s="50"/>
+      <c r="R23" s="50"/>
+      <c r="S23" s="50"/>
+      <c r="T23" s="50"/>
+      <c r="U23" s="50"/>
       <c r="X23" t="s">
         <v>70</v>
       </c>
@@ -2525,16 +2946,16 @@
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
       <c r="M24" s="13"/>
-      <c r="P24" s="61" t="s">
+      <c r="P24" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="Q24" s="61"/>
-      <c r="R24" s="61"/>
-      <c r="S24" s="61" t="s">
+      <c r="Q24" s="51"/>
+      <c r="R24" s="51"/>
+      <c r="S24" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="T24" s="61"/>
-      <c r="U24" s="61"/>
+      <c r="T24" s="51"/>
+      <c r="U24" s="51"/>
       <c r="X24" s="3" t="s">
         <v>62</v>
       </c>
@@ -2554,12 +2975,12 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
-      <c r="P25" s="60"/>
-      <c r="Q25" s="60"/>
-      <c r="R25" s="60"/>
-      <c r="S25" s="60"/>
-      <c r="T25" s="60"/>
-      <c r="U25" s="60"/>
+      <c r="P25" s="50"/>
+      <c r="Q25" s="50"/>
+      <c r="R25" s="50"/>
+      <c r="S25" s="50"/>
+      <c r="T25" s="50"/>
+      <c r="U25" s="50"/>
       <c r="X25" t="s">
         <v>63</v>
       </c>
@@ -2569,30 +2990,30 @@
       </c>
     </row>
     <row r="26" spans="1:26" ht="18" x14ac:dyDescent="0.4">
-      <c r="B26" s="101" t="s">
+      <c r="B26" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="101"/>
-      <c r="D26" s="101"/>
-      <c r="E26" s="101"/>
-      <c r="F26" s="101"/>
-      <c r="G26" s="101"/>
-      <c r="H26" s="101"/>
-      <c r="I26" s="101"/>
-      <c r="J26" s="101"/>
-      <c r="K26" s="101"/>
-      <c r="L26" s="101"/>
-      <c r="M26" s="101"/>
-      <c r="P26" s="60" t="s">
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="75"/>
+      <c r="H26" s="75"/>
+      <c r="I26" s="75"/>
+      <c r="J26" s="75"/>
+      <c r="K26" s="75"/>
+      <c r="L26" s="75"/>
+      <c r="M26" s="75"/>
+      <c r="P26" s="50" t="s">
         <v>115</v>
       </c>
-      <c r="Q26" s="60"/>
-      <c r="R26" s="60" t="s">
+      <c r="Q26" s="50"/>
+      <c r="R26" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="S26" s="60"/>
-      <c r="T26" s="60"/>
-      <c r="U26" s="60"/>
+      <c r="S26" s="50"/>
+      <c r="T26" s="50"/>
+      <c r="U26" s="50"/>
       <c r="X26" s="3" t="s">
         <v>64</v>
       </c>
@@ -2602,26 +3023,26 @@
       </c>
     </row>
     <row r="27" spans="1:26" s="18" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="102"/>
-      <c r="C27" s="102"/>
-      <c r="D27" s="102"/>
-      <c r="E27" s="102"/>
-      <c r="F27" s="102"/>
-      <c r="G27" s="102"/>
-      <c r="H27" s="102"/>
-      <c r="I27" s="102"/>
-      <c r="J27" s="102"/>
-      <c r="K27" s="102"/>
-      <c r="L27" s="102"/>
-      <c r="M27" s="102"/>
-      <c r="P27" s="61" t="s">
+      <c r="B27" s="79"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="79"/>
+      <c r="H27" s="79"/>
+      <c r="I27" s="79"/>
+      <c r="J27" s="79"/>
+      <c r="K27" s="79"/>
+      <c r="L27" s="79"/>
+      <c r="M27" s="79"/>
+      <c r="P27" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="Q27" s="157"/>
-      <c r="R27" s="157"/>
-      <c r="S27" s="157"/>
-      <c r="T27" s="157"/>
-      <c r="U27" s="157"/>
+      <c r="Q27" s="54"/>
+      <c r="R27" s="54"/>
+      <c r="S27" s="54"/>
+      <c r="T27" s="54"/>
+      <c r="U27" s="54"/>
       <c r="X27" s="18" t="s">
         <v>71</v>
       </c>
@@ -2647,14 +3068,14 @@
       <c r="L28" s="17"/>
       <c r="M28" s="17"/>
       <c r="N28" s="17"/>
-      <c r="P28" s="61" t="s">
+      <c r="P28" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="Q28" s="60"/>
-      <c r="R28" s="60"/>
-      <c r="S28" s="60"/>
-      <c r="T28" s="60"/>
-      <c r="U28" s="60"/>
+      <c r="Q28" s="50"/>
+      <c r="R28" s="50"/>
+      <c r="S28" s="50"/>
+      <c r="T28" s="50"/>
+      <c r="U28" s="50"/>
       <c r="X28" t="s">
         <v>65</v>
       </c>
@@ -2680,14 +3101,14 @@
       <c r="M29" s="19"/>
       <c r="N29" s="19"/>
       <c r="O29" s="9"/>
-      <c r="P29" s="61" t="s">
+      <c r="P29" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="Q29" s="61"/>
-      <c r="R29" s="61"/>
-      <c r="S29" s="61"/>
-      <c r="T29" s="61"/>
-      <c r="U29" s="61"/>
+      <c r="Q29" s="51"/>
+      <c r="R29" s="51"/>
+      <c r="S29" s="51"/>
+      <c r="T29" s="51"/>
+      <c r="U29" s="51"/>
       <c r="X29" s="3" t="s">
         <v>75</v>
       </c>
@@ -2789,21 +3210,21 @@
     </row>
     <row r="33" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="22"/>
-      <c r="B33" s="103" t="s">
+      <c r="B33" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="103"/>
-      <c r="D33" s="103"/>
+      <c r="C33" s="80"/>
+      <c r="D33" s="80"/>
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
       <c r="G33" s="1"/>
       <c r="H33" s="22"/>
       <c r="I33" s="22"/>
-      <c r="J33" s="103" t="s">
+      <c r="J33" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="K33" s="103"/>
-      <c r="L33" s="103"/>
+      <c r="K33" s="80"/>
+      <c r="L33" s="80"/>
       <c r="M33" s="22"/>
       <c r="N33" s="22"/>
       <c r="O33" s="1"/>
@@ -2817,29 +3238,29 @@
       <c r="U33" s="17"/>
     </row>
     <row r="34" spans="1:21" s="3" customFormat="1" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="104" t="s">
+      <c r="A34" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="104"/>
-      <c r="C34" s="104"/>
-      <c r="D34" s="104"/>
-      <c r="E34" s="104"/>
-      <c r="F34" s="104"/>
+      <c r="B34" s="76"/>
+      <c r="C34" s="76"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="76"/>
       <c r="G34" s="9"/>
-      <c r="H34" s="104" t="s">
+      <c r="H34" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="I34" s="104"/>
-      <c r="J34" s="104"/>
-      <c r="K34" s="104"/>
-      <c r="L34" s="104"/>
-      <c r="M34" s="104"/>
-      <c r="N34" s="104"/>
+      <c r="I34" s="76"/>
+      <c r="J34" s="76"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="76"/>
+      <c r="M34" s="76"/>
+      <c r="N34" s="76"/>
       <c r="O34" s="9"/>
-      <c r="P34" s="105" t="s">
+      <c r="P34" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="Q34" s="105"/>
+      <c r="Q34" s="77"/>
       <c r="R34" s="15"/>
       <c r="S34" s="15"/>
       <c r="T34" s="15"/>
@@ -2856,20 +3277,20 @@
       <c r="U35" s="17"/>
     </row>
     <row r="36" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="99"/>
-      <c r="B36" s="99"/>
-      <c r="C36" s="99"/>
-      <c r="D36" s="99"/>
-      <c r="E36" s="99"/>
-      <c r="F36" s="99"/>
-      <c r="G36" s="99"/>
-      <c r="H36" s="99"/>
-      <c r="I36" s="99"/>
-      <c r="J36" s="99"/>
-      <c r="K36" s="99"/>
-      <c r="L36" s="99"/>
-      <c r="M36" s="99"/>
-      <c r="N36" s="99"/>
+      <c r="A36" s="78"/>
+      <c r="B36" s="78"/>
+      <c r="C36" s="78"/>
+      <c r="D36" s="78"/>
+      <c r="E36" s="78"/>
+      <c r="F36" s="78"/>
+      <c r="G36" s="78"/>
+      <c r="H36" s="78"/>
+      <c r="I36" s="78"/>
+      <c r="J36" s="78"/>
+      <c r="K36" s="78"/>
+      <c r="L36" s="78"/>
+      <c r="M36" s="78"/>
+      <c r="N36" s="78"/>
       <c r="P36" s="14" t="s">
         <v>32</v>
       </c>
@@ -2880,22 +3301,22 @@
       <c r="U36" s="17"/>
     </row>
     <row r="37" spans="1:21" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="101" t="s">
+      <c r="A37" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="101"/>
-      <c r="C37" s="101"/>
-      <c r="D37" s="101"/>
-      <c r="E37" s="101"/>
-      <c r="F37" s="101"/>
-      <c r="G37" s="101"/>
-      <c r="H37" s="101"/>
-      <c r="I37" s="101"/>
-      <c r="J37" s="101"/>
-      <c r="K37" s="101"/>
-      <c r="L37" s="101"/>
-      <c r="M37" s="101"/>
-      <c r="N37" s="101"/>
+      <c r="B37" s="75"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="75"/>
+      <c r="H37" s="75"/>
+      <c r="I37" s="75"/>
+      <c r="J37" s="75"/>
+      <c r="K37" s="75"/>
+      <c r="L37" s="75"/>
+      <c r="M37" s="75"/>
+      <c r="N37" s="75"/>
       <c r="P37" s="25" t="s">
         <v>34</v>
       </c>
@@ -2958,16 +3379,16 @@
       <c r="L40" s="20"/>
       <c r="M40" s="20"/>
       <c r="N40" s="20"/>
-      <c r="P40" s="99" t="s">
+      <c r="P40" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="Q40" s="99"/>
-      <c r="R40" s="99"/>
-      <c r="S40" s="99" t="s">
+      <c r="Q40" s="78"/>
+      <c r="R40" s="78"/>
+      <c r="S40" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="T40" s="99"/>
-      <c r="U40" s="99"/>
+      <c r="T40" s="78"/>
+      <c r="U40" s="78"/>
     </row>
     <row r="41" spans="1:21" ht="18" x14ac:dyDescent="0.4">
       <c r="A41" s="23"/>
@@ -2986,38 +3407,66 @@
       <c r="L41" s="27"/>
       <c r="M41" s="27"/>
       <c r="N41" s="27"/>
-      <c r="P41" s="101" t="s">
+      <c r="P41" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="Q41" s="101"/>
-      <c r="R41" s="101"/>
-      <c r="S41" s="101" t="s">
+      <c r="Q41" s="75"/>
+      <c r="R41" s="75"/>
+      <c r="S41" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="T41" s="101"/>
-      <c r="U41" s="101"/>
+      <c r="T41" s="75"/>
+      <c r="U41" s="75"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="80">
-    <mergeCell ref="P41:R41"/>
-    <mergeCell ref="S41:U41"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="H34:N34"/>
-    <mergeCell ref="P34:Q34"/>
-    <mergeCell ref="A36:N36"/>
-    <mergeCell ref="A37:N37"/>
-    <mergeCell ref="P40:R40"/>
-    <mergeCell ref="B26:M26"/>
-    <mergeCell ref="B27:M27"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="S40:U40"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="A16:M16"/>
-    <mergeCell ref="P17:U17"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="Q10:T10"/>
+    <mergeCell ref="Q6:T6"/>
+    <mergeCell ref="Q8:T8"/>
+    <mergeCell ref="Q11:T11"/>
+    <mergeCell ref="Q5:T5"/>
+    <mergeCell ref="Q7:T7"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A3:N3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="K4:K6"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="N4:N8"/>
+    <mergeCell ref="O4:O8"/>
+    <mergeCell ref="M9:M11"/>
+    <mergeCell ref="P7:P9"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J9:J11"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="Q13:T13"/>
@@ -3034,52 +3483,24 @@
     <mergeCell ref="K9:K11"/>
     <mergeCell ref="L9:L11"/>
     <mergeCell ref="I12:I13"/>
-    <mergeCell ref="M9:M11"/>
-    <mergeCell ref="P7:P9"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="J9:J11"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="N4:N8"/>
-    <mergeCell ref="O4:O8"/>
-    <mergeCell ref="A3:N3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="I4:I6"/>
-    <mergeCell ref="J4:J6"/>
-    <mergeCell ref="K4:K6"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="Q10:T10"/>
-    <mergeCell ref="Q6:T6"/>
-    <mergeCell ref="Q8:T8"/>
-    <mergeCell ref="Q11:T11"/>
-    <mergeCell ref="Q5:T5"/>
-    <mergeCell ref="Q7:T7"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="A16:M16"/>
+    <mergeCell ref="P17:U17"/>
+    <mergeCell ref="B26:M26"/>
+    <mergeCell ref="B27:M27"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="S40:U40"/>
+    <mergeCell ref="P41:R41"/>
+    <mergeCell ref="S41:U41"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="H34:N34"/>
+    <mergeCell ref="P34:Q34"/>
+    <mergeCell ref="A36:N36"/>
+    <mergeCell ref="A37:N37"/>
+    <mergeCell ref="P40:R40"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0" footer="0"/>
@@ -3093,8 +3514,8 @@
   <sheetPr codeName="Sheet127"/>
   <dimension ref="B2:N33"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="175" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:E19"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="175" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="17.25" x14ac:dyDescent="0.4"/>
@@ -3113,573 +3534,527 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="133" t="s">
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="131" t="s">
         <v>94</v>
       </c>
-      <c r="H2" s="133"/>
-      <c r="I2" s="133"/>
-      <c r="J2" s="133"/>
-      <c r="K2" s="133"/>
-      <c r="L2" s="133"/>
-      <c r="M2" s="133"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131"/>
+      <c r="M2" s="131"/>
     </row>
     <row r="3" spans="2:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="136" t="s">
+      <c r="B3" s="161" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="136"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="136"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="161"/>
+      <c r="E3" s="161"/>
     </row>
     <row r="4" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="139" t="s">
+      <c r="B4" s="119" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="141" t="s">
+      <c r="C4" s="121" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="142"/>
-      <c r="E4" s="42" t="s">
+      <c r="D4" s="122"/>
+      <c r="E4" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="G4" s="146" t="s">
+      <c r="G4" s="144" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="131" t="s">
+      <c r="H4" s="171" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="131"/>
-      <c r="J4" s="131" t="s">
+      <c r="I4" s="172"/>
+      <c r="J4" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="131"/>
-      <c r="L4" s="131"/>
-      <c r="M4" s="148"/>
+      <c r="K4" s="142"/>
+      <c r="L4" s="142"/>
+      <c r="M4" s="143"/>
     </row>
     <row r="5" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="140"/>
-      <c r="C5" s="67">
+      <c r="B5" s="120"/>
+      <c r="C5" s="53">
         <v>1</v>
       </c>
-      <c r="D5" s="67">
+      <c r="D5" s="53">
         <v>2</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="G5" s="147"/>
-      <c r="H5" s="132"/>
-      <c r="I5" s="132"/>
-      <c r="J5" s="37">
+      <c r="G5" s="145"/>
+      <c r="H5" s="173"/>
+      <c r="I5" s="174"/>
+      <c r="J5" s="65">
         <v>1</v>
       </c>
-      <c r="K5" s="37">
+      <c r="K5" s="65">
         <v>2</v>
       </c>
-      <c r="L5" s="37">
+      <c r="L5" s="65">
         <v>3</v>
       </c>
-      <c r="M5" s="39">
+      <c r="M5" s="66">
         <v>4</v>
       </c>
-      <c r="N5" s="49"/>
-    </row>
-    <row r="6" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="64"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="66"/>
-      <c r="G6" s="135" t="s">
+      <c r="N5" s="68"/>
+    </row>
+    <row r="6" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="52"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="56"/>
+      <c r="G6" s="162" t="s">
         <v>107</v>
       </c>
-      <c r="H6" s="134" t="s">
+      <c r="H6" s="167" t="s">
         <v>108</v>
       </c>
-      <c r="I6" s="134"/>
-      <c r="J6" s="112"/>
-      <c r="K6" s="112"/>
-      <c r="L6" s="112"/>
-      <c r="M6" s="114"/>
-    </row>
-    <row r="7" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="44"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="45"/>
-      <c r="G7" s="135"/>
-      <c r="H7" s="134"/>
-      <c r="I7" s="134"/>
-      <c r="J7" s="113"/>
-      <c r="K7" s="113"/>
-      <c r="L7" s="113"/>
-      <c r="M7" s="115"/>
-    </row>
-    <row r="8" spans="2:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="44"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="45"/>
-      <c r="G8" s="135"/>
-      <c r="H8" s="134" t="s">
+      <c r="I6" s="168"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="126"/>
+      <c r="L6" s="126"/>
+      <c r="M6" s="124"/>
+    </row>
+    <row r="7" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="40"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="57"/>
+      <c r="G7" s="163"/>
+      <c r="H7" s="169"/>
+      <c r="I7" s="170"/>
+      <c r="J7" s="127"/>
+      <c r="K7" s="127"/>
+      <c r="L7" s="127"/>
+      <c r="M7" s="125"/>
+    </row>
+    <row r="8" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="41"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="59"/>
+      <c r="G8" s="164"/>
+      <c r="H8" s="165" t="s">
         <v>95</v>
       </c>
-      <c r="I8" s="134"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="40"/>
-    </row>
-    <row r="9" spans="2:14" ht="11.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="46"/>
-      <c r="C9" s="149"/>
-      <c r="D9" s="149"/>
-      <c r="E9" s="151"/>
-      <c r="G9" s="123" t="s">
+      <c r="I8" s="166"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="37"/>
+    </row>
+    <row r="9" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="69"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="71"/>
+      <c r="G9" s="139" t="s">
         <v>96</v>
       </c>
-      <c r="H9" s="138" t="s">
+      <c r="H9" s="135" t="s">
         <v>97</v>
       </c>
-      <c r="I9" s="138"/>
-      <c r="J9" s="112"/>
-      <c r="K9" s="112"/>
-      <c r="L9" s="112"/>
-      <c r="M9" s="114"/>
-    </row>
-    <row r="10" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="47"/>
-      <c r="C10" s="150"/>
-      <c r="D10" s="150"/>
-      <c r="E10" s="152"/>
-      <c r="G10" s="123"/>
-      <c r="H10" s="138"/>
+      <c r="I9" s="136"/>
+      <c r="J9" s="126"/>
+      <c r="K9" s="126"/>
+      <c r="L9" s="126"/>
+      <c r="M9" s="124"/>
+    </row>
+    <row r="10" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="72"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="74"/>
+      <c r="G10" s="146"/>
+      <c r="H10" s="137"/>
       <c r="I10" s="138"/>
-      <c r="J10" s="113"/>
-      <c r="K10" s="113"/>
-      <c r="L10" s="113"/>
-      <c r="M10" s="115"/>
-    </row>
-    <row r="11" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="44"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="45"/>
-      <c r="G11" s="123"/>
-      <c r="H11" s="138" t="s">
+      <c r="J10" s="127"/>
+      <c r="K10" s="127"/>
+      <c r="L10" s="127"/>
+      <c r="M10" s="125"/>
+    </row>
+    <row r="11" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="40"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="57"/>
+      <c r="G11" s="146"/>
+      <c r="H11" s="135" t="s">
         <v>109</v>
       </c>
-      <c r="I11" s="138"/>
-      <c r="J11" s="112"/>
-      <c r="K11" s="112"/>
-      <c r="L11" s="112"/>
-      <c r="M11" s="114"/>
-    </row>
-    <row r="12" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="44"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="45"/>
-      <c r="G12" s="123"/>
-      <c r="H12" s="138"/>
+      <c r="I11" s="136"/>
+      <c r="J11" s="126"/>
+      <c r="K11" s="126"/>
+      <c r="L11" s="126"/>
+      <c r="M11" s="124"/>
+    </row>
+    <row r="12" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="40"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="57"/>
+      <c r="G12" s="140"/>
+      <c r="H12" s="137"/>
       <c r="I12" s="138"/>
-      <c r="J12" s="113"/>
-      <c r="K12" s="113"/>
-      <c r="L12" s="113"/>
-      <c r="M12" s="115"/>
-    </row>
-    <row r="13" spans="2:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="44"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="45"/>
-      <c r="G13" s="123" t="s">
+      <c r="J12" s="127"/>
+      <c r="K12" s="127"/>
+      <c r="L12" s="127"/>
+      <c r="M12" s="125"/>
+    </row>
+    <row r="13" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="40"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="57"/>
+      <c r="G13" s="139" t="s">
         <v>98</v>
       </c>
-      <c r="H13" s="138" t="s">
+      <c r="H13" s="135" t="s">
         <v>110</v>
       </c>
-      <c r="I13" s="138"/>
-      <c r="J13" s="112"/>
-      <c r="K13" s="112"/>
-      <c r="L13" s="112"/>
-      <c r="M13" s="114"/>
+      <c r="I13" s="136"/>
+      <c r="J13" s="126"/>
+      <c r="K13" s="126"/>
+      <c r="L13" s="126"/>
+      <c r="M13" s="124"/>
     </row>
     <row r="14" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="64"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="66"/>
-      <c r="G14" s="123"/>
-      <c r="H14" s="138"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="56"/>
+      <c r="G14" s="140"/>
+      <c r="H14" s="137"/>
       <c r="I14" s="138"/>
-      <c r="J14" s="113"/>
-      <c r="K14" s="113"/>
-      <c r="L14" s="113"/>
-      <c r="M14" s="115"/>
+      <c r="J14" s="127"/>
+      <c r="K14" s="127"/>
+      <c r="L14" s="127"/>
+      <c r="M14" s="125"/>
     </row>
     <row r="15" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="44"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="45"/>
-      <c r="G15" s="123" t="s">
+      <c r="B15" s="40"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="57"/>
+      <c r="G15" s="139" t="s">
         <v>99</v>
       </c>
-      <c r="H15" s="121" t="s">
+      <c r="H15" s="148" t="s">
         <v>100</v>
       </c>
-      <c r="I15" s="121"/>
-      <c r="J15" s="112"/>
-      <c r="K15" s="112"/>
-      <c r="L15" s="112"/>
-      <c r="M15" s="114"/>
-    </row>
-    <row r="16" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="44"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="45"/>
-      <c r="G16" s="123"/>
-      <c r="H16" s="121"/>
-      <c r="I16" s="121"/>
-      <c r="J16" s="137"/>
-      <c r="K16" s="137"/>
-      <c r="L16" s="137"/>
-      <c r="M16" s="155"/>
-    </row>
-    <row r="17" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="44"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="45"/>
-      <c r="G17" s="123"/>
-      <c r="H17" s="121"/>
-      <c r="I17" s="121"/>
-      <c r="J17" s="113"/>
-      <c r="K17" s="113"/>
-      <c r="L17" s="113"/>
-      <c r="M17" s="115"/>
+      <c r="I15" s="149"/>
+      <c r="J15" s="126"/>
+      <c r="K15" s="126"/>
+      <c r="L15" s="126"/>
+      <c r="M15" s="124"/>
+    </row>
+    <row r="16" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="40"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="57"/>
+      <c r="G16" s="146"/>
+      <c r="H16" s="152"/>
+      <c r="I16" s="153"/>
+      <c r="J16" s="130"/>
+      <c r="K16" s="130"/>
+      <c r="L16" s="130"/>
+      <c r="M16" s="129"/>
+    </row>
+    <row r="17" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="40"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="57"/>
+      <c r="G17" s="146"/>
+      <c r="H17" s="154"/>
+      <c r="I17" s="155"/>
+      <c r="J17" s="127"/>
+      <c r="K17" s="127"/>
+      <c r="L17" s="127"/>
+      <c r="M17" s="125"/>
     </row>
     <row r="18" spans="2:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="143" t="s">
+      <c r="B18" s="116" t="s">
         <v>106</v>
       </c>
-      <c r="C18" s="144"/>
-      <c r="D18" s="145"/>
-      <c r="E18" s="48"/>
-      <c r="G18" s="123"/>
-      <c r="H18" s="121" t="s">
+      <c r="C18" s="117"/>
+      <c r="D18" s="118"/>
+      <c r="E18" s="42"/>
+      <c r="G18" s="146"/>
+      <c r="H18" s="148" t="s">
         <v>111</v>
       </c>
-      <c r="I18" s="121"/>
-      <c r="J18" s="112"/>
-      <c r="K18" s="112"/>
-      <c r="L18" s="112"/>
-      <c r="M18" s="114"/>
+      <c r="I18" s="149"/>
+      <c r="J18" s="126"/>
+      <c r="K18" s="126"/>
+      <c r="L18" s="126"/>
+      <c r="M18" s="124"/>
     </row>
     <row r="19" spans="2:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="136" t="s">
+      <c r="B19" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="136"/>
-      <c r="D19" s="136"/>
-      <c r="E19" s="136"/>
-      <c r="G19" s="124"/>
-      <c r="H19" s="122"/>
-      <c r="I19" s="122"/>
-      <c r="J19" s="154"/>
-      <c r="K19" s="154"/>
-      <c r="L19" s="154"/>
-      <c r="M19" s="153"/>
+      <c r="C19" s="123"/>
+      <c r="D19" s="123"/>
+      <c r="E19" s="123"/>
+      <c r="G19" s="147"/>
+      <c r="H19" s="150"/>
+      <c r="I19" s="151"/>
+      <c r="J19" s="128"/>
+      <c r="K19" s="128"/>
+      <c r="L19" s="128"/>
+      <c r="M19" s="134"/>
     </row>
     <row r="20" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="139" t="s">
+      <c r="B20" s="119" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="141" t="s">
+      <c r="C20" s="121" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="142"/>
-      <c r="E20" s="42" t="s">
+      <c r="D20" s="122"/>
+      <c r="E20" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="G20" s="116" t="s">
+      <c r="G20" s="156" t="s">
         <v>101</v>
       </c>
-      <c r="H20" s="117"/>
-      <c r="I20" s="118"/>
+      <c r="H20" s="157"/>
+      <c r="I20" s="158"/>
     </row>
     <row r="21" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="140"/>
-      <c r="C21" s="67">
+      <c r="B21" s="120"/>
+      <c r="C21" s="53">
         <v>3</v>
       </c>
-      <c r="D21" s="67">
+      <c r="D21" s="53">
         <v>4</v>
       </c>
-      <c r="E21" s="43" t="s">
+      <c r="E21" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="41" t="s">
+      <c r="G21" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="H21" s="120" t="s">
+      <c r="H21" s="159" t="s">
         <v>102</v>
       </c>
-      <c r="I21" s="125"/>
-    </row>
-    <row r="22" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="64"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="65"/>
-      <c r="E22" s="66"/>
-      <c r="G22" s="50" t="s">
+      <c r="I21" s="160"/>
+    </row>
+    <row r="22" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="52"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="56"/>
+      <c r="G22" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="H22" s="106" t="s">
+      <c r="H22" s="132" t="s">
         <v>103</v>
       </c>
-      <c r="I22" s="107"/>
-    </row>
-    <row r="23" spans="2:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="44"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="45"/>
-      <c r="G23" s="50" t="s">
+      <c r="I22" s="133"/>
+    </row>
+    <row r="23" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="40"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="57"/>
+      <c r="G23" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="H23" s="106" t="s">
+      <c r="H23" s="132" t="s">
         <v>52</v>
       </c>
-      <c r="I23" s="107"/>
-    </row>
-    <row r="24" spans="2:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="44"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="45"/>
-      <c r="G24" s="50" t="s">
+      <c r="I23" s="133"/>
+    </row>
+    <row r="24" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="40"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="57"/>
+      <c r="G24" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="H24" s="106" t="s">
+      <c r="H24" s="132" t="s">
         <v>56</v>
       </c>
-      <c r="I24" s="107"/>
-    </row>
-    <row r="25" spans="2:13" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="44"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="45"/>
-      <c r="G25" s="53" t="s">
+      <c r="I24" s="133"/>
+    </row>
+    <row r="25" spans="2:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B25" s="40"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="57"/>
+      <c r="G25" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="H25" s="129" t="s">
+      <c r="H25" s="177" t="s">
         <v>60</v>
       </c>
-      <c r="I25" s="130"/>
-    </row>
-    <row r="26" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="44"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="45"/>
-      <c r="G26" s="126" t="s">
+      <c r="I25" s="178"/>
+    </row>
+    <row r="26" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="40"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="57"/>
+      <c r="G26" s="156" t="s">
         <v>104</v>
       </c>
-      <c r="H26" s="127"/>
-      <c r="I26" s="127"/>
-      <c r="J26" s="127"/>
-      <c r="K26" s="127"/>
-      <c r="L26" s="127"/>
-      <c r="M26" s="128"/>
-    </row>
-    <row r="27" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="44"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="45"/>
-      <c r="G27" s="119" t="s">
+      <c r="H26" s="157"/>
+      <c r="I26" s="157"/>
+      <c r="J26" s="157"/>
+      <c r="K26" s="157"/>
+      <c r="L26" s="157"/>
+      <c r="M26" s="158"/>
+    </row>
+    <row r="27" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="40"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="57"/>
+      <c r="G27" s="175" t="s">
         <v>105</v>
       </c>
-      <c r="H27" s="120"/>
-      <c r="I27" s="37" t="s">
+      <c r="H27" s="176"/>
+      <c r="I27" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="J27" s="120" t="s">
+      <c r="J27" s="159" t="s">
         <v>1</v>
       </c>
-      <c r="K27" s="120"/>
-      <c r="L27" s="120"/>
-      <c r="M27" s="125"/>
-    </row>
-    <row r="28" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="44"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="45"/>
-      <c r="G28" s="108" t="s">
+      <c r="K27" s="180"/>
+      <c r="L27" s="180"/>
+      <c r="M27" s="160"/>
+    </row>
+    <row r="28" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="40"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="57"/>
+      <c r="G28" s="181" t="s">
         <v>42</v>
       </c>
-      <c r="H28" s="106"/>
-      <c r="I28" s="51" t="s">
+      <c r="H28" s="182"/>
+      <c r="I28" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="J28" s="106" t="s">
+      <c r="J28" s="132" t="s">
         <v>44</v>
       </c>
-      <c r="K28" s="106"/>
-      <c r="L28" s="106"/>
-      <c r="M28" s="107"/>
-    </row>
-    <row r="29" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="64"/>
-      <c r="C29" s="65"/>
-      <c r="D29" s="65"/>
-      <c r="E29" s="66"/>
-      <c r="G29" s="108" t="s">
+      <c r="K28" s="179"/>
+      <c r="L28" s="179"/>
+      <c r="M28" s="133"/>
+    </row>
+    <row r="29" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B29" s="52"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="56"/>
+      <c r="G29" s="181" t="s">
         <v>46</v>
       </c>
-      <c r="H29" s="106"/>
-      <c r="I29" s="51" t="s">
+      <c r="H29" s="182"/>
+      <c r="I29" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="J29" s="106" t="s">
+      <c r="J29" s="132" t="s">
         <v>44</v>
       </c>
-      <c r="K29" s="106"/>
-      <c r="L29" s="106"/>
-      <c r="M29" s="107"/>
-    </row>
-    <row r="30" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="44"/>
-      <c r="C30" s="63"/>
-      <c r="D30" s="63"/>
-      <c r="E30" s="45"/>
-      <c r="G30" s="108" t="s">
+      <c r="K29" s="179"/>
+      <c r="L29" s="179"/>
+      <c r="M29" s="133"/>
+    </row>
+    <row r="30" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="40"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="57"/>
+      <c r="G30" s="181" t="s">
         <v>49</v>
       </c>
-      <c r="H30" s="106"/>
-      <c r="I30" s="51" t="s">
+      <c r="H30" s="182"/>
+      <c r="I30" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="J30" s="106" t="s">
+      <c r="J30" s="132" t="s">
         <v>44</v>
       </c>
-      <c r="K30" s="106"/>
-      <c r="L30" s="106"/>
-      <c r="M30" s="107"/>
-    </row>
-    <row r="31" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="44"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="45"/>
-      <c r="G31" s="108" t="s">
+      <c r="K30" s="179"/>
+      <c r="L30" s="179"/>
+      <c r="M30" s="133"/>
+    </row>
+    <row r="31" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="40"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="57"/>
+      <c r="G31" s="181" t="s">
         <v>53</v>
       </c>
-      <c r="H31" s="106"/>
-      <c r="I31" s="51" t="s">
+      <c r="H31" s="182"/>
+      <c r="I31" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="J31" s="106" t="s">
+      <c r="J31" s="132" t="s">
         <v>44</v>
       </c>
-      <c r="K31" s="106"/>
-      <c r="L31" s="106"/>
-      <c r="M31" s="107"/>
-    </row>
-    <row r="32" spans="2:13" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="44"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="45"/>
-      <c r="G32" s="111" t="s">
+      <c r="K31" s="179"/>
+      <c r="L31" s="179"/>
+      <c r="M31" s="133"/>
+    </row>
+    <row r="32" spans="2:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B32" s="40"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="57"/>
+      <c r="G32" s="183" t="s">
         <v>112</v>
       </c>
-      <c r="H32" s="109"/>
-      <c r="I32" s="52" t="s">
+      <c r="H32" s="184"/>
+      <c r="I32" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="J32" s="109" t="s">
+      <c r="J32" s="177" t="s">
         <v>58</v>
       </c>
-      <c r="K32" s="109"/>
-      <c r="L32" s="109"/>
-      <c r="M32" s="110"/>
+      <c r="K32" s="185"/>
+      <c r="L32" s="185"/>
+      <c r="M32" s="178"/>
     </row>
     <row r="33" spans="2:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B33" s="143" t="s">
+      <c r="B33" s="116" t="s">
         <v>106</v>
       </c>
-      <c r="C33" s="144"/>
-      <c r="D33" s="145"/>
-      <c r="E33" s="48"/>
+      <c r="C33" s="117"/>
+      <c r="D33" s="118"/>
+      <c r="E33" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="70">
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H11:I12"/>
-    <mergeCell ref="H13:I14"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="H9:I10"/>
-    <mergeCell ref="G9:G12"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="K15:K17"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="L13:L14"/>
+  <mergeCells count="67">
+    <mergeCell ref="J30:M30"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="J31:M31"/>
+    <mergeCell ref="J32:M32"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G32:H32"/>
     <mergeCell ref="J29:M29"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="M15:M17"/>
-    <mergeCell ref="L15:L17"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="H4:I5"/>
-    <mergeCell ref="G2:M2"/>
-    <mergeCell ref="H6:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G26:M26"/>
-    <mergeCell ref="J27:M27"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="H15:I17"/>
-    <mergeCell ref="H18:I19"/>
-    <mergeCell ref="G15:G19"/>
-    <mergeCell ref="H21:I21"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:K7"/>
@@ -3689,13 +4064,56 @@
     <mergeCell ref="L11:L12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J30:M30"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="J31:M31"/>
-    <mergeCell ref="J32:M32"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G26:M26"/>
+    <mergeCell ref="J27:M27"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G9:G12"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="H4:I5"/>
+    <mergeCell ref="G2:M2"/>
+    <mergeCell ref="H6:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="M15:M17"/>
+    <mergeCell ref="L15:L17"/>
+    <mergeCell ref="H9:I10"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="H15:I17"/>
+    <mergeCell ref="H18:I19"/>
+    <mergeCell ref="G15:G19"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H11:I12"/>
+    <mergeCell ref="H13:I14"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="J9:J10"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0" footer="0"/>

</xml_diff>